<commit_message>
Added special cards, tweaks to AI, WebGL test build, changed to play card system to support abilities, started on card selection system, added cover image to AI cards
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AIValues.xlsx
+++ b/Assets/StreamingAssets/AIValues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\pazaak\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D53187-40C2-41A9-842C-3363608BAF1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8BB21D-010C-4C39-90F2-56D626FAAA66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36543D9A-7390-4D61-821D-32AEFC4914B9}"/>
   </bookViews>
@@ -68,15 +68,23 @@
     <t>Holly</t>
   </si>
   <si>
-    <t>5,6,7,8,9,5,6,7,8,9</t>
+    <t>N|5,N|6,N|7,N|8,N|9,N|5,N|6,N|7,N|8,N|9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,16 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4084DC-0835-402F-8357-BE0AFDE4AC94}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,7 +510,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Basic opponent selection screen, using imported value, basic sprite import system currrent just for AI profile images, some UI tweaks
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AIValues.xlsx
+++ b/Assets/StreamingAssets/AIValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\pazaak\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8BB21D-010C-4C39-90F2-56D626FAAA66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B1D9FE-B17F-49BF-A554-801F627EFCCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36543D9A-7390-4D61-821D-32AEFC4914B9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Difficulty</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>N|5,N|6,N|7,N|8,N|9,N|5,N|6,N|7,N|8,N|9</t>
+  </si>
+  <si>
+    <t>SpirteName</t>
+  </si>
+  <si>
+    <t>AI01.png</t>
+  </si>
+  <si>
+    <t>AI02.png</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,9 +449,10 @@
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +468,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -475,8 +488,11 @@
       <c r="E2">
         <v>50</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -492,8 +508,11 @@
       <c r="E3">
         <v>25</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -508,6 +527,9 @@
       </c>
       <c r="E4">
         <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added card shop, tweaks to how player deck is saved, added cradtis to AI
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AIValues.xlsx
+++ b/Assets/StreamingAssets/AIValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\pazaak\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B1D9FE-B17F-49BF-A554-801F627EFCCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0799B1-F2D9-4106-A531-5C17355654E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36543D9A-7390-4D61-821D-32AEFC4914B9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Difficulty</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>AI02.png</t>
+  </si>
+  <si>
+    <t>Credits</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +455,7 @@
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +474,11 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -491,8 +497,11 @@
       <c r="F2" t="s">
         <v>13</v>
       </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -511,8 +520,11 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
+      <c r="G3">
+        <v>250</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -530,6 +542,9 @@
       </c>
       <c r="F4" t="s">
         <v>13</v>
+      </c>
+      <c r="G4">
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bug fixes to card selection, bought cards now appear, new AI images and bug fix
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AIValues.xlsx
+++ b/Assets/StreamingAssets/AIValues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\pazaak\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0799B1-F2D9-4106-A531-5C17355654E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D320918B-138E-4F7B-B55C-71EC11E8AF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36543D9A-7390-4D61-821D-32AEFC4914B9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Difficulty</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Skynet</t>
   </si>
   <si>
-    <t>Microsoft Sam</t>
-  </si>
-  <si>
     <t>Holly</t>
   </si>
   <si>
@@ -74,13 +71,22 @@
     <t>SpirteName</t>
   </si>
   <si>
-    <t>AI01.png</t>
-  </si>
-  <si>
-    <t>AI02.png</t>
-  </si>
-  <si>
     <t>Credits</t>
+  </si>
+  <si>
+    <t>N|5,N|6,N|7,N|8,N|9,N|-5,N|-6,N|-7,N|-8,N|-9</t>
+  </si>
+  <si>
+    <t>Sam.png</t>
+  </si>
+  <si>
+    <t>Holly.png</t>
+  </si>
+  <si>
+    <t>Skynet.png</t>
+  </si>
+  <si>
+    <t>MS Sam</t>
   </si>
 </sst>
 </file>
@@ -444,15 +450,16 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -472,10 +479,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -483,19 +490,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
         <v>11</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -506,10 +513,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -518,7 +525,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>250</v>
@@ -532,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -541,7 +548,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <v>500</v>

</xml_diff>

<commit_message>
Fix to character creator, changed betting to use odds, added new betting screen, some UI tweaks
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AIValues.xlsx
+++ b/Assets/StreamingAssets/AIValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\pazaak\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D320918B-138E-4F7B-B55C-71EC11E8AF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6223D0-7D7F-4D3C-AD57-D4774CF355EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36543D9A-7390-4D61-821D-32AEFC4914B9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Difficulty</t>
   </si>
@@ -71,9 +71,6 @@
     <t>SpirteName</t>
   </si>
   <si>
-    <t>Credits</t>
-  </si>
-  <si>
     <t>N|5,N|6,N|7,N|8,N|9,N|-5,N|-6,N|-7,N|-8,N|-9</t>
   </si>
   <si>
@@ -87,6 +84,18 @@
   </si>
   <si>
     <t>MS Sam</t>
+  </si>
+  <si>
+    <t>Odds</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1,25</t>
+  </si>
+  <si>
+    <t>1,5</t>
   </si>
 </sst>
 </file>
@@ -130,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +460,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -490,7 +500,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -502,10 +512,10 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -525,10 +535,10 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>250</v>
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -539,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -548,10 +558,10 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4">
-        <v>500</v>
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>